<commit_message>
phonemes coverage works fine
</commit_message>
<xml_diff>
--- a/src/main/java/output/PhonemesCoverage.xlsx
+++ b/src/main/java/output/PhonemesCoverage.xlsx
@@ -1432,7 +1432,7 @@
       <c r="B3" t="s">
         <v>81</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="18">
         <v>72</v>
       </c>
       <c r="E3" t="s">
@@ -1444,25 +1444,25 @@
       <c r="J3" t="s">
         <v>84</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="18">
         <v>73</v>
       </c>
       <c r="N3" t="s">
         <v>102</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" t="s" s="18">
         <v>103</v>
       </c>
       <c r="P3" t="s">
         <v>149</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" t="s" s="18">
         <v>150</v>
       </c>
       <c r="R3" t="s">
         <v>151</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" t="s" s="18">
         <v>152</v>
       </c>
       <c r="U3" t="s">
@@ -1477,47 +1477,47 @@
       <c r="A4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="18">
         <v>77</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="18">
         <v>78</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="18">
         <v>75</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="18">
         <v>80</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="18">
         <v>100</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" t="s" s="18">
         <v>101</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" t="s" s="18">
         <v>88</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" t="s" s="18">
         <v>154</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" t="s" s="18">
         <v>155</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" t="s" s="18">
         <v>156</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" t="s" s="18">
         <v>157</v>
       </c>
-      <c r="U4" t="s">
+      <c r="U4" t="s" s="18">
         <v>158</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V4" t="s" s="18">
         <v>159</v>
       </c>
       <c r="W4" s="15"/>
-      <c r="X4" t="s">
+      <c r="X4" t="s" s="18">
         <v>160</v>
       </c>
       <c r="Y4" s="15"/>
@@ -1532,7 +1532,7 @@
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="18">
         <v>94</v>
       </c>
       <c r="K5" t="s">
@@ -1541,7 +1541,7 @@
       <c r="L5" t="s">
         <v>96</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="18">
         <v>97</v>
       </c>
       <c r="N5" t="s">
@@ -1625,28 +1625,28 @@
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="18">
         <v>74</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" t="s" s="18">
         <v>114</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="s" s="18">
         <v>115</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" t="s" s="18">
         <v>116</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" t="s" s="18">
         <v>117</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" t="s" s="18">
         <v>118</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" t="s" s="18">
         <v>171</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" t="s" s="18">
         <v>172</v>
       </c>
       <c r="R7" s="15"/>
@@ -1662,16 +1662,16 @@
       <c r="A8" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="18">
         <v>85</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="18">
         <v>86</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="18">
         <v>87</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="18">
         <v>89</v>
       </c>
       <c r="F8" s="16" t="s">
@@ -1680,10 +1680,10 @@
       <c r="G8" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="18" t="s">
         <v>122</v>
       </c>
       <c r="J8" s="17" t="s">
@@ -1701,34 +1701,34 @@
       <c r="O8" t="s">
         <v>127</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" t="s" s="18">
         <v>173</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8" t="s" s="18">
         <v>174</v>
       </c>
-      <c r="R8" s="16" t="s">
+      <c r="R8" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="S8" s="16" t="s">
+      <c r="S8" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="T8" s="16" t="s">
+      <c r="T8" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="U8" s="16" t="s">
+      <c r="U8" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="V8" s="16" t="s">
+      <c r="V8" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="W8" s="16" t="s">
+      <c r="W8" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="X8" s="16" t="s">
+      <c r="X8" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="Y8" s="16" t="s">
+      <c r="Y8" s="18" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1757,7 +1757,7 @@
       <c r="P9" t="s">
         <v>184</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" t="s" s="18">
         <v>183</v>
       </c>
       <c r="R9" s="16" t="s">
@@ -1819,7 +1819,7 @@
       <c r="J11" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="K11" s="18" t="s">
         <v>79</v>
       </c>
       <c r="N11" t="s">
@@ -1833,13 +1833,13 @@
       <c r="T11" t="s">
         <v>190</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U11" t="s" s="18">
         <v>189</v>
       </c>
       <c r="V11" t="s">
         <v>188</v>
       </c>
-      <c r="W11" t="s">
+      <c r="W11" t="s" s="18">
         <v>187</v>
       </c>
       <c r="X11" s="15"/>
@@ -1924,13 +1924,13 @@
       <c r="J14" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="K14" s="18" t="s">
         <v>76</v>
       </c>
       <c r="N14" t="s">
         <v>208</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O14" t="s" s="18">
         <v>207</v>
       </c>
       <c r="P14" t="s">

</xml_diff>